<commit_message>
Finished the Hierarchy Traversal Test section.
</commit_message>
<xml_diff>
--- a/article/thesis_tests_n8.xlsx
+++ b/article/thesis_tests_n8.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="893"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="893" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="office-n8-d2" sheetId="49" r:id="rId1"/>
@@ -922,7 +922,7 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="B1:AU36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I14" sqref="I14:J14"/>
     </sheetView>
   </sheetViews>
@@ -2908,9 +2908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AV68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6942,8 +6940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AU36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11:M11"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG11" sqref="AG11:AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8929,9 +8927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AU39"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14:AA14"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11138,8 +11134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AV74"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V55" sqref="V55:AA55"/>
+    <sheetView topLeftCell="S7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC39" sqref="AC39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11649,7 +11645,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="52">
-        <f t="shared" ref="D11" si="0">$N11-$I11</f>
+        <f>$N11-$I11</f>
         <v>644610</v>
       </c>
       <c r="E11" s="53"/>
@@ -13679,7 +13675,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="52">
-        <f t="shared" ref="D48" si="1">$N48-$I48</f>
+        <f t="shared" ref="D48" si="0">$N48-$I48</f>
         <v>2225287</v>
       </c>
       <c r="E48" s="53"/>
@@ -14437,7 +14433,7 @@
       <c r="G62" s="77"/>
       <c r="H62" s="77"/>
       <c r="I62" s="71">
-        <f t="shared" ref="I62:I71" si="2">SUM($AO62:$AP62)</f>
+        <f t="shared" ref="I62:I71" si="1">SUM($AO62:$AP62)</f>
         <v>18565461</v>
       </c>
       <c r="J62" s="71"/>
@@ -14461,7 +14457,7 @@
       <c r="Z62" s="77"/>
       <c r="AA62" s="77"/>
       <c r="AB62" s="71">
-        <f t="shared" ref="AB62:AB74" si="3">SUM($AR62:$AS62)</f>
+        <f t="shared" ref="AB62:AB74" si="2">SUM($AR62:$AS62)</f>
         <v>9947518</v>
       </c>
       <c r="AC62" s="71"/>
@@ -14503,7 +14499,7 @@
       <c r="G63" s="77"/>
       <c r="H63" s="77"/>
       <c r="I63" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6525475</v>
       </c>
       <c r="J63" s="71"/>
@@ -14527,7 +14523,7 @@
       <c r="Z63" s="77"/>
       <c r="AA63" s="77"/>
       <c r="AB63" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5088286</v>
       </c>
       <c r="AC63" s="71"/>
@@ -14569,7 +14565,7 @@
       <c r="G64" s="77"/>
       <c r="H64" s="77"/>
       <c r="I64" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>811008</v>
       </c>
       <c r="J64" s="71"/>
@@ -14593,7 +14589,7 @@
       <c r="Z64" s="77"/>
       <c r="AA64" s="77"/>
       <c r="AB64" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>614052</v>
       </c>
       <c r="AC64" s="71"/>
@@ -14635,7 +14631,7 @@
       <c r="G65" s="77"/>
       <c r="H65" s="77"/>
       <c r="I65" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1304</v>
       </c>
       <c r="J65" s="71"/>
@@ -14659,7 +14655,7 @@
       <c r="Z65" s="77"/>
       <c r="AA65" s="77"/>
       <c r="AB65" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>96126</v>
       </c>
       <c r="AC65" s="71"/>
@@ -14701,7 +14697,7 @@
       <c r="G66" s="77"/>
       <c r="H66" s="77"/>
       <c r="I66" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>809704</v>
       </c>
       <c r="J66" s="71"/>
@@ -14725,7 +14721,7 @@
       <c r="Z66" s="77"/>
       <c r="AA66" s="77"/>
       <c r="AB66" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>517926</v>
       </c>
       <c r="AC66" s="71"/>
@@ -14767,7 +14763,7 @@
       <c r="G67" s="77"/>
       <c r="H67" s="77"/>
       <c r="I67" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6477632</v>
       </c>
       <c r="J67" s="71"/>
@@ -14791,7 +14787,7 @@
       <c r="Z67" s="77"/>
       <c r="AA67" s="77"/>
       <c r="AB67" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4143408</v>
       </c>
       <c r="AC67" s="71"/>
@@ -14833,7 +14829,7 @@
       <c r="G68" s="77"/>
       <c r="H68" s="77"/>
       <c r="I68" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4252345</v>
       </c>
       <c r="J68" s="71"/>
@@ -14857,7 +14853,7 @@
       <c r="Z68" s="77"/>
       <c r="AA68" s="77"/>
       <c r="AB68" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2858615</v>
       </c>
       <c r="AC68" s="71"/>
@@ -14899,7 +14895,7 @@
       <c r="G69" s="77"/>
       <c r="H69" s="77"/>
       <c r="I69" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2225287</v>
       </c>
       <c r="J69" s="71"/>
@@ -14923,7 +14919,7 @@
       <c r="Z69" s="77"/>
       <c r="AA69" s="77"/>
       <c r="AB69" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1284793</v>
       </c>
       <c r="AC69" s="71"/>
@@ -14965,7 +14961,7 @@
       <c r="G70" s="77"/>
       <c r="H70" s="77"/>
       <c r="I70" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>17802296</v>
       </c>
       <c r="J70" s="71"/>
@@ -14989,7 +14985,7 @@
       <c r="Z70" s="77"/>
       <c r="AA70" s="77"/>
       <c r="AB70" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>10278344</v>
       </c>
       <c r="AC70" s="71"/>
@@ -15031,7 +15027,7 @@
       <c r="G71" s="77"/>
       <c r="H71" s="77"/>
       <c r="I71" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14311812</v>
       </c>
       <c r="J71" s="71"/>
@@ -15055,7 +15051,7 @@
       <c r="Z71" s="77"/>
       <c r="AA71" s="77"/>
       <c r="AB71" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6992777</v>
       </c>
       <c r="AC71" s="71"/>
@@ -15121,7 +15117,7 @@
       <c r="Z72" s="77"/>
       <c r="AA72" s="77"/>
       <c r="AB72" s="71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3285567</v>
       </c>
       <c r="AC72" s="71"/>
@@ -15253,7 +15249,7 @@
       <c r="Z74" s="65"/>
       <c r="AA74" s="65"/>
       <c r="AB74" s="66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>41320340</v>
       </c>
       <c r="AC74" s="66"/>
@@ -15571,7 +15567,7 @@
   <dimension ref="B1:AU39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="W12" sqref="W12:AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17779,8 +17775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AU43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13:AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20258,8 +20254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AV82"/>
   <sheetViews>
-    <sheetView topLeftCell="C37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V60" sqref="V60:AA60"/>
+    <sheetView topLeftCell="T40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W54" sqref="W54:AA54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25247,9 +25243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AU43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:R5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>